<commit_message>
Marcar clausulas repetidas en CBC temporal
</commit_message>
<xml_diff>
--- a/Python/ExcelTemp.xlsx
+++ b/Python/ExcelTemp.xlsx
@@ -1,50 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Requierements Temp" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Requierements Temp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>Id_Req</t>
+  </si>
+  <si>
+    <t>Desc_Req</t>
+  </si>
+  <si>
+    <t>ID_Req_BBDD</t>
+  </si>
+  <si>
+    <t>Descr_Req_BBDD</t>
+  </si>
+  <si>
+    <t>%Coincidencia</t>
+  </si>
+  <si>
+    <t>Resp_BBDD</t>
+  </si>
+  <si>
+    <t>Coment_BBDD</t>
+  </si>
+  <si>
+    <t>Nueva_Respuesta</t>
+  </si>
+  <si>
+    <t>Nuevos_comentarios</t>
+  </si>
+  <si>
+    <t>EFB-RS-703</t>
+  </si>
+  <si>
+    <t>EFB-RS-704</t>
+  </si>
+  <si>
+    <t>Dampers shall activated before a tunnel entrance by the train control unit. This functionality will be defined during the project phase.</t>
+  </si>
+  <si>
+    <t>Dampers control strategy shall ensure dampers can be closed before entering a tunnel</t>
+  </si>
+  <si>
+    <t>EFB-RS-707</t>
+  </si>
+  <si>
+    <t>EFB-RS-708</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>HC_230517: Acording to CAF instructions, pressure wave proteccions only apply to MD, not to P2 CER</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -74,88 +123,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -443,139 +421,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Id_Req</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Desc_Req</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ID_Req_BBDD</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Descr_Req_BBDD</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>%Coincidencia</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Resp_BBDD</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Coment_BBDD</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Nueva_Respuesta</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>Nuevos_comentarios</t>
-        </is>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>EFB-RS-703</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Dampers shall activated before a tunnel entrance by the train control unit. This functionality will be defined during the project phase.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>EFB-RS-707</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Dampers shall activated before a tunnel entrance by the train control unit. This functionality will be defined during the project phase.</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
         <v>100</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>HC_230517: Acording to CAF instructions, pressure wave proteccions only apply to MD, not to P2 CER</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>EFB-RS-704</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Dampers control strategy shall ensure dampers can be closed before entering a tunnel</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>EFB-RS-708</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Dampers control strategy shall ensure dampers can be closed before entering a tunnel</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>100</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>HC_230517: Acording to CAF instructions, pressure wave proteccions only apply to MD, not to P2 CER</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Adaptada LoadDatabase a SQL Server - Acceso por pwd a LoadFromTemp
</commit_message>
<xml_diff>
--- a/Python/ExcelTemp.xlsx
+++ b/Python/ExcelTemp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Id_Req</t>
   </si>
@@ -40,7 +40,13 @@
     <t>Nueva_Respuesta</t>
   </si>
   <si>
-    <t>Nuevos_comentarios</t>
+    <t>Nuevos_Comentarios</t>
+  </si>
+  <si>
+    <t>Proyecto_Origen</t>
+  </si>
+  <si>
+    <t>Fichero_Origen</t>
   </si>
   <si>
     <t>EFB-RS-703</t>
@@ -65,6 +71,12 @@
   </si>
   <si>
     <t>HC_230517: Acording to CAF instructions, pressure wave proteccions only apply to MD, not to P2 CER</t>
+  </si>
+  <si>
+    <t>CERCANÍAS RENFE</t>
+  </si>
+  <si>
+    <t>EFFAE CBC SALA CERCANIA.xlsx</t>
   </si>
 </sst>
 </file>
@@ -422,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,51 +468,69 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>